<commit_message>
diagram and classview treated
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PFavatoBarcelos\Dev\Work\ontouml-json2graph\tests\test_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB54A3BE-EDA0-42DA-BDDA-436D34088089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82A6DA5-F16C-4D39-83A2-D1C45FDDFC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
@@ -183,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -197,12 +197,31 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -281,33 +300,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I13" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I13" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:I13" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{B2169228-FA5D-41A3-ABA5-DC9D70D992D5}" name="Description"/>
-    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="8">
+    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="10">
       <calculatedColumnFormula>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="7">
+    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="9">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".vpp"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="8">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".json"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="7">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".ttl"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -603,16 +622,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BB1B56-C601-4BA2-9A5D-7647C7ECF9E4}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="61.5703125" customWidth="1"/>
+    <col min="2" max="2" width="68.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" hidden="1" customWidth="1"/>
     <col min="4" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="73.5703125" bestFit="1" customWidth="1"/>
@@ -903,29 +922,28 @@
       <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="5" t="str">
+      <c r="C10" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_009</v>
       </c>
-      <c r="D10" s="5" t="str">
+      <c r="D10" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_009.vpp</v>
       </c>
-      <c r="E10" s="5" t="str">
+      <c r="E10" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_009.json</v>
       </c>
-      <c r="F10" s="5" t="str">
+      <c r="F10" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_009.ttl</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="5"/>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -934,29 +952,28 @@
       <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="5" t="str">
+      <c r="C11" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_010</v>
       </c>
-      <c r="D11" s="5" t="str">
+      <c r="D11" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_010.vpp</v>
       </c>
-      <c r="E11" s="5" t="str">
+      <c r="E11" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_010.json</v>
       </c>
-      <c r="F11" s="5" t="str">
+      <c r="F11" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_010.ttl</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" s="5"/>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -965,29 +982,28 @@
       <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="5" t="str">
+      <c r="C12" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_011</v>
       </c>
-      <c r="D12" s="5" t="str">
+      <c r="D12" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_011.vpp</v>
       </c>
-      <c r="E12" s="5" t="str">
+      <c r="E12" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_011.json</v>
       </c>
-      <c r="F12" s="5" t="str">
+      <c r="F12" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_011.ttl</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="5"/>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -996,42 +1012,41 @@
       <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="5" t="str">
+      <c r="C13" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_012</v>
       </c>
-      <c r="D13" s="5" t="str">
+      <c r="D13" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_012.vpp</v>
       </c>
-      <c r="E13" s="5" t="str">
+      <c r="E13" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_012.json</v>
       </c>
-      <c r="F13" s="5" t="str">
+      <c r="F13" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_012.ttl</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="5"/>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1050,7 +1065,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
new test added (still without .tll file)
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82A6DA5-F16C-4D39-83A2-D1C45FDDFC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA67DC9-37E8-489D-90F0-DDE1C466B845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>#</t>
   </si>
@@ -123,6 +112,12 @@
   </si>
   <si>
     <t>011 + class outside diagram</t>
+  </si>
+  <si>
+    <t>same class twice in the same diagram</t>
+  </si>
+  <si>
+    <t>012 + multiple classes of stereotype type and collective</t>
   </si>
 </sst>
 </file>
@@ -183,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -197,6 +192,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -300,8 +296,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I13" totalsRowShown="0" headerRowDxfId="12">
-  <autoFilter ref="A1:I13" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I14" totalsRowShown="0" headerRowDxfId="12">
+  <autoFilter ref="A1:I14" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{B2169228-FA5D-41A3-ABA5-DC9D70D992D5}" name="Description"/>
@@ -622,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BB1B56-C601-4BA2-9A5D-7647C7ECF9E4}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,10 +785,10 @@
         <v>test_004.ttl</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -819,10 +815,10 @@
         <v>test_005.ttl</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -849,10 +845,10 @@
         <v>test_006.ttl</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -879,10 +875,10 @@
         <v>test_007.ttl</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -909,10 +905,10 @@
         <v>test_008.ttl</v>
       </c>
       <c r="G9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -939,10 +935,10 @@
         <v>test_009.ttl</v>
       </c>
       <c r="G10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1035,32 +1031,68 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_013</v>
+      </c>
+      <c r="D14" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_013.vpp</v>
+      </c>
+      <c r="E14" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_013.json</v>
+      </c>
+      <c r="F14" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_013.ttl</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:H13">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="G2:H14">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H13" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H14" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
       <formula1>"Done,TBD"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
test_015 added and working
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA67DC9-37E8-489D-90F0-DDE1C466B845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEE9339-AF0B-4997-8E70-761F85BB45BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>#</t>
   </si>
@@ -51,9 +51,6 @@
     <t>graph2json</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Project only.</t>
   </si>
   <si>
@@ -118,6 +115,12 @@
   </si>
   <si>
     <t>012 + multiple classes of stereotype type and collective</t>
+  </si>
+  <si>
+    <t>014 + examples of classes non-collective with isExtensional true</t>
+  </si>
+  <si>
+    <t>013 + classes with multiple stereotypes</t>
   </si>
 </sst>
 </file>
@@ -178,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -192,12 +195,33 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -296,26 +320,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I14" totalsRowShown="0" headerRowDxfId="12">
-  <autoFilter ref="A1:I14" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I16" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="A1:I16" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{B2169228-FA5D-41A3-ABA5-DC9D70D992D5}" name="Description"/>
-    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="10">
+    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="12">
       <calculatedColumnFormula>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="9">
+    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="11">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".vpp"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="8">
+    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="10">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".json"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="7">
+    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="9">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".ttl"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -621,7 +645,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +683,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -667,7 +691,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -686,13 +710,13 @@
         <v>test_001.ttl</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -700,7 +724,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -719,13 +743,13 @@
         <v>test_002.ttl</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -733,32 +757,32 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_003</v>
+      </c>
+      <c r="D4" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_003.vpp</v>
+      </c>
+      <c r="E4" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_003.json</v>
+      </c>
+      <c r="F4" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_003.ttl</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="str">
-        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
-        <v>test_003</v>
-      </c>
-      <c r="D4" t="str">
-        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
-        <v>test_003.vpp</v>
-      </c>
-      <c r="E4" t="str">
-        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
-        <v>test_003.json</v>
-      </c>
-      <c r="F4" t="str">
-        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
-        <v>test_003.ttl</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -766,7 +790,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -785,10 +809,10 @@
         <v>test_004.ttl</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -796,7 +820,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -815,10 +839,10 @@
         <v>test_005.ttl</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -826,7 +850,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -845,10 +869,10 @@
         <v>test_006.ttl</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -856,7 +880,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -875,10 +899,10 @@
         <v>test_007.ttl</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -886,7 +910,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -905,10 +929,10 @@
         <v>test_008.ttl</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -916,7 +940,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -934,11 +958,11 @@
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_009.ttl</v>
       </c>
-      <c r="G10" t="s">
-        <v>10</v>
+      <c r="G10" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="H10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -946,7 +970,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -965,10 +989,10 @@
         <v>test_010.ttl</v>
       </c>
       <c r="G11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -976,7 +1000,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -995,10 +1019,10 @@
         <v>test_011.ttl</v>
       </c>
       <c r="G12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1006,7 +1030,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1025,10 +1049,10 @@
         <v>test_012.ttl</v>
       </c>
       <c r="G13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1036,63 +1060,124 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_013</v>
+      </c>
+      <c r="D14" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_013.vpp</v>
+      </c>
+      <c r="E14" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_013.json</v>
+      </c>
+      <c r="F14" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_013.ttl</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="6" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_014</v>
+      </c>
+      <c r="D15" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_014.vpp</v>
+      </c>
+      <c r="E15" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_014.json</v>
+      </c>
+      <c r="F15" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_014.ttl</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="5" t="str">
-        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
-        <v>test_013</v>
-      </c>
-      <c r="D14" s="5" t="str">
-        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
-        <v>test_013.vpp</v>
-      </c>
-      <c r="E14" s="5" t="str">
-        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
-        <v>test_013.json</v>
-      </c>
-      <c r="F14" s="5" t="str">
-        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
-        <v>test_013.ttl</v>
-      </c>
-      <c r="G14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="5"/>
+      <c r="C16" s="6" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_015</v>
+      </c>
+      <c r="D16" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_015.vpp</v>
+      </c>
+      <c r="E16" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_015.json</v>
+      </c>
+      <c r="F16" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_015.ttl</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="6"/>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:H14">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="G2:H16">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H14" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H16" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
       <formula1>"Done,TBD"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
test_016 added and working
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEE9339-AF0B-4997-8E70-761F85BB45BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B74F9D1-F6FA-4790-997D-4DFE2F9032F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>#</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>013 + classes with multiple stereotypes</t>
+  </si>
+  <si>
+    <t>015 + examples of classes unaligned isPowertype and stereotype</t>
   </si>
 </sst>
 </file>
@@ -201,7 +204,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -320,26 +333,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I16" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="A1:I16" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I17" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:I17" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{B2169228-FA5D-41A3-ABA5-DC9D70D992D5}" name="Description"/>
-    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="13">
       <calculatedColumnFormula>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="12">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".vpp"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="10">
+    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="11">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".json"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="9">
+    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="10">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".ttl"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -645,7 +658,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,9 +725,6 @@
       <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
       <c r="I2" t="s">
         <v>15</v>
       </c>
@@ -745,9 +755,6 @@
       <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
       <c r="I3" t="s">
         <v>14</v>
       </c>
@@ -778,9 +785,6 @@
       <c r="G4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
       <c r="I4" t="s">
         <v>12</v>
       </c>
@@ -811,9 +815,6 @@
       <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -841,9 +842,6 @@
       <c r="G6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -871,9 +869,6 @@
       <c r="G7" t="s">
         <v>9</v>
       </c>
-      <c r="H7" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -901,9 +896,6 @@
       <c r="G8" t="s">
         <v>9</v>
       </c>
-      <c r="H8" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -931,9 +923,6 @@
       <c r="G9" t="s">
         <v>9</v>
       </c>
-      <c r="H9" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -958,10 +947,7 @@
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_009.ttl</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="G10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -991,9 +977,6 @@
       <c r="G11" t="s">
         <v>9</v>
       </c>
-      <c r="H11" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1021,9 +1004,6 @@
       <c r="G12" t="s">
         <v>9</v>
       </c>
-      <c r="H12" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1051,9 +1031,6 @@
       <c r="G13" t="s">
         <v>9</v>
       </c>
-      <c r="H13" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1081,40 +1058,33 @@
       <c r="G14" t="s">
         <v>9</v>
       </c>
-      <c r="H14" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="6" t="str">
+      <c r="C15" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_014</v>
       </c>
-      <c r="D15" s="6" t="str">
+      <c r="D15" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_014.vpp</v>
       </c>
-      <c r="E15" s="6" t="str">
+      <c r="E15" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_014.json</v>
       </c>
-      <c r="F15" s="6" t="str">
+      <c r="F15" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_014.ttl</v>
       </c>
       <c r="G15" t="s">
         <v>9</v>
       </c>
-      <c r="H15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1123,31 +1093,55 @@
       <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="6" t="str">
+      <c r="C16" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_015</v>
       </c>
-      <c r="D16" s="6" t="str">
+      <c r="D16" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_015.vpp</v>
       </c>
-      <c r="E16" s="6" t="str">
+      <c r="E16" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_015.json</v>
       </c>
-      <c r="F16" s="6" t="str">
+      <c r="F16" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_015.ttl</v>
       </c>
       <c r="G16" t="s">
         <v>9</v>
       </c>
-      <c r="H16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="6" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_016</v>
+      </c>
+      <c r="D17" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_016.vpp</v>
+      </c>
+      <c r="E17" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_016.json</v>
+      </c>
+      <c r="F17" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_016.ttl</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>21</v>
       </c>
@@ -1168,16 +1162,19 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:H16">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+  <conditionalFormatting sqref="G2:H17">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A17">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H16" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H17" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
       <formula1>"Done,TBD"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
test_017 added and working
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B74F9D1-F6FA-4790-997D-4DFE2F9032F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC3715F-F42E-4122-97AD-DB5A9AA2820A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>#</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>015 + examples of classes unaligned isPowertype and stereotype</t>
+  </si>
+  <si>
+    <t>016 + examples of constraints B and C of validate_class_constraints</t>
   </si>
 </sst>
 </file>
@@ -184,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -198,13 +201,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -217,16 +229,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -252,16 +254,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -333,26 +325,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I17" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A1:I17" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I18" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="A1:I18" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{B2169228-FA5D-41A3-ABA5-DC9D70D992D5}" name="Description"/>
-    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="13">
+    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="12">
       <calculatedColumnFormula>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="12">
+    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="11">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".vpp"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="10">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".json"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="10">
+    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="9">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".ttl"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -658,7 +650,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,26 +1112,54 @@
       <c r="B17" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="6" t="str">
+      <c r="C17" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_016</v>
       </c>
-      <c r="D17" s="6" t="str">
+      <c r="D17" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_016.vpp</v>
       </c>
-      <c r="E17" s="6" t="str">
+      <c r="E17" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_016.json</v>
       </c>
-      <c r="F17" s="6" t="str">
+      <c r="F17" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_016.ttl</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" s="6"/>
+      <c r="G17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_017</v>
+      </c>
+      <c r="D18" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_017.vpp</v>
+      </c>
+      <c r="E18" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_017.json</v>
+      </c>
+      <c r="F18" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_017.ttl</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
@@ -1162,7 +1182,10 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:H17">
+  <conditionalFormatting sqref="A2:A18">
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:H18">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
@@ -1170,11 +1193,8 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A17">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H17" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H18" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
       <formula1>"Done,TBD"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added tests 18 and 19 - both working
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC3715F-F42E-4122-97AD-DB5A9AA2820A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C649BCB-B9ED-4445-8E79-F1BAF4AB74DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>#</t>
   </si>
@@ -90,9 +90,6 @@
     <t>007 + diagram on package's package</t>
   </si>
   <si>
-    <t>class in two different diagrams</t>
-  </si>
-  <si>
     <t>test multiple projects in a single JSON file</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>011 + class outside diagram</t>
   </si>
   <si>
-    <t>same class twice in the same diagram</t>
-  </si>
-  <si>
     <t>012 + multiple classes of stereotype type and collective</t>
   </si>
   <si>
@@ -127,6 +121,12 @@
   </si>
   <si>
     <t>016 + examples of constraints B and C of validate_class_constraints</t>
+  </si>
+  <si>
+    <t>Same class in two different diagrams</t>
+  </si>
+  <si>
+    <t>018 + same class twice in the same diagram</t>
   </si>
 </sst>
 </file>
@@ -187,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -202,11 +202,42 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -325,26 +356,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I18" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="A1:I18" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I20" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A1:I20" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{B2169228-FA5D-41A3-ABA5-DC9D70D992D5}" name="Description"/>
-    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="15">
       <calculatedColumnFormula>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="14">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".vpp"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="10">
+    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="13">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".json"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="9">
+    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="12">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".ttl"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -647,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BB1B56-C601-4BA2-9A5D-7647C7ECF9E4}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,7 +952,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -948,7 +979,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -975,7 +1006,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1002,7 +1033,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1029,7 +1060,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1056,7 +1087,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1083,7 +1114,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1110,7 +1141,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1137,64 +1168,110 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_017</v>
+      </c>
+      <c r="D18" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_017.vpp</v>
+      </c>
+      <c r="E18" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_017.json</v>
+      </c>
+      <c r="F18" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_017.ttl</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_018</v>
+      </c>
+      <c r="D19" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_018.vpp</v>
+      </c>
+      <c r="E19" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_018.json</v>
+      </c>
+      <c r="F19" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_018.ttl</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="5" t="str">
-        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
-        <v>test_017</v>
-      </c>
-      <c r="D18" s="5" t="str">
-        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
-        <v>test_017.vpp</v>
-      </c>
-      <c r="E18" s="5" t="str">
-        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
-        <v>test_017.json</v>
-      </c>
-      <c r="F18" s="5" t="str">
-        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
-        <v>test_017.ttl</v>
-      </c>
-      <c r="G18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>21</v>
-      </c>
+      <c r="C20" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_019</v>
+      </c>
+      <c r="D20" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_019.vpp</v>
+      </c>
+      <c r="E20" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_019.json</v>
+      </c>
+      <c r="F20" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_019.ttl</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A18">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+  <conditionalFormatting sqref="A2:A20">
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H18">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+  <conditionalFormatting sqref="G2:H20">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H18" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H20" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
       <formula1>"Done,TBD"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added tests 20 to 23 (not tested yet)
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C649BCB-B9ED-4445-8E79-F1BAF4AB74DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E24F5B-E551-462C-97F1-C94EA322FB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>#</t>
   </si>
@@ -127,6 +127,24 @@
   </si>
   <si>
     <t>018 + same class twice in the same diagram</t>
+  </si>
+  <si>
+    <t>020 + added class attributes of diverse types</t>
+  </si>
+  <si>
+    <t>019 + added class attributes</t>
+  </si>
+  <si>
+    <t>021 + added class attributes with diverse multiplicities</t>
+  </si>
+  <si>
+    <t>022 + multiple different properties for attributes</t>
+  </si>
+  <si>
+    <t>add generalization</t>
+  </si>
+  <si>
+    <t>add relation</t>
   </si>
 </sst>
 </file>
@@ -136,7 +154,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +173,14 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -187,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -203,11 +229,72 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -356,26 +443,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I20" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="A1:I20" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I24" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:I24" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{B2169228-FA5D-41A3-ABA5-DC9D70D992D5}" name="Description"/>
-    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="15">
+    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="21">
       <calculatedColumnFormula>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="14">
+    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="20">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".vpp"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="13">
+    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="19">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".json"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="12">
+    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="18">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".ttl"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -678,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BB1B56-C601-4BA2-9A5D-7647C7ECF9E4}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,27 +1284,25 @@
       <c r="B19" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="5" t="str">
+      <c r="C19" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_018</v>
       </c>
-      <c r="D19" s="5" t="str">
+      <c r="D19" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_018.vpp</v>
       </c>
-      <c r="E19" s="5" t="str">
+      <c r="E19" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_018.json</v>
       </c>
-      <c r="F19" s="5" t="str">
+      <c r="F19" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_018.ttl</v>
       </c>
       <c r="G19" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -1226,27 +1311,133 @@
       <c r="B20" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="5" t="str">
+      <c r="C20" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_019</v>
       </c>
-      <c r="D20" s="6" t="str">
+      <c r="D20" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_019.vpp</v>
       </c>
-      <c r="E20" s="5" t="str">
+      <c r="E20" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_019.json</v>
       </c>
-      <c r="F20" s="6" t="str">
+      <c r="F20" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_019.ttl</v>
       </c>
       <c r="G20" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_020</v>
+      </c>
+      <c r="D21" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_020.vpp</v>
+      </c>
+      <c r="E21" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_020.json</v>
+      </c>
+      <c r="F21" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_020.ttl</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_021</v>
+      </c>
+      <c r="D22" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_021.vpp</v>
+      </c>
+      <c r="E22" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_021.json</v>
+      </c>
+      <c r="F22" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_021.ttl</v>
+      </c>
+      <c r="G22" s="6"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_022</v>
+      </c>
+      <c r="D23" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_022.vpp</v>
+      </c>
+      <c r="E23" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_022.json</v>
+      </c>
+      <c r="F23" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_022.ttl</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_023</v>
+      </c>
+      <c r="D24" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_023.vpp</v>
+      </c>
+      <c r="E24" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_023.json</v>
+      </c>
+      <c r="F24" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_023.ttl</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
@@ -1258,20 +1449,33 @@
         <v>22</v>
       </c>
     </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="7"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A20">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+  <conditionalFormatting sqref="A2:A24">
+    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H20">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+  <conditionalFormatting sqref="G2:H24">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H20" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H24" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
       <formula1>"Done,TBD"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
tests 21 and 22 working. test 23 improved.
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E24F5B-E551-462C-97F1-C94EA322FB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F8B835-3FAB-47BC-94A8-18594F19E7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t>#</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>add relation</t>
+  </si>
+  <si>
+    <t>add enumerations</t>
   </si>
 </sst>
 </file>
@@ -154,7 +157,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,14 +176,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -213,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -227,134 +222,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -443,26 +316,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I24" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I24" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:I24" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{B2169228-FA5D-41A3-ABA5-DC9D70D992D5}" name="Description"/>
-    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="21">
+    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="9">
       <calculatedColumnFormula>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="20">
+    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="8">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".vpp"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="19">
+    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="7">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".json"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="18">
+    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="6">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".ttl"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -768,7 +641,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,7 +1096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1250,7 +1123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1277,7 +1150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1304,7 +1177,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1331,116 +1204,113 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="5" t="str">
+      <c r="C21" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_020</v>
       </c>
-      <c r="D21" s="5" t="str">
+      <c r="D21" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_020.vpp</v>
       </c>
-      <c r="E21" s="5" t="str">
+      <c r="E21" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_020.json</v>
       </c>
-      <c r="F21" s="5" t="str">
+      <c r="F21" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_020.ttl</v>
       </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="5" t="str">
+      <c r="C22" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_021</v>
       </c>
-      <c r="D22" s="5" t="str">
+      <c r="D22" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_021.vpp</v>
       </c>
-      <c r="E22" s="5" t="str">
+      <c r="E22" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_021.json</v>
       </c>
-      <c r="F22" s="5" t="str">
+      <c r="F22" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_021.ttl</v>
       </c>
-      <c r="G22" s="6"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="5" t="str">
+      <c r="C23" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_022</v>
       </c>
-      <c r="D23" s="5" t="str">
+      <c r="D23" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_022.vpp</v>
       </c>
-      <c r="E23" s="5" t="str">
+      <c r="E23" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_022.json</v>
       </c>
-      <c r="F23" s="5" t="str">
+      <c r="F23" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_022.ttl</v>
       </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G23" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="5" t="str">
+      <c r="C24" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_023</v>
       </c>
-      <c r="D24" s="5" t="str">
+      <c r="D24" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_023.vpp</v>
       </c>
-      <c r="E24" s="5" t="str">
+      <c r="E24" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_023.json</v>
       </c>
-      <c r="F24" s="5" t="str">
+      <c r="F24" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_023.ttl</v>
       </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="B33" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1451,26 +1321,28 @@
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A24">
-    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:H24">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
tests 24 and 25 working
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F8B835-3FAB-47BC-94A8-18594F19E7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9921A52-0563-4F09-8823-04049C217963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>#</t>
   </si>
@@ -90,12 +90,6 @@
     <t>007 + diagram on package's package</t>
   </si>
   <si>
-    <t>test multiple projects in a single JSON file</t>
-  </si>
-  <si>
-    <t>adds diagrams inside different ModelElements</t>
-  </si>
-  <si>
     <t>008 + class inside diagram</t>
   </si>
   <si>
@@ -148,6 +142,21 @@
   </si>
   <si>
     <t>add enumerations</t>
+  </si>
+  <si>
+    <t>add subsets and redefines to properties</t>
+  </si>
+  <si>
+    <t>add stereotypes for properties</t>
+  </si>
+  <si>
+    <t>add text box, notes, and comments</t>
+  </si>
+  <si>
+    <t>023 + added attributes's stereotypes (single, valid, invalid, multiple, etc.) and meta-properties</t>
+  </si>
+  <si>
+    <t>024 + added text boxes, notes and elements' comments</t>
   </si>
 </sst>
 </file>
@@ -208,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -223,11 +232,72 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -316,26 +386,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I24" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:I24" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I26" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A1:I26" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{B2169228-FA5D-41A3-ABA5-DC9D70D992D5}" name="Description"/>
-    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="9">
+    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="15">
       <calculatedColumnFormula>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="8">
+    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="14">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".vpp"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="13">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".json"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="6">
+    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="12">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".ttl"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -638,22 +708,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BB1B56-C601-4BA2-9A5D-7647C7ECF9E4}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="68.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="4" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="73.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="68.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" hidden="1" customWidth="1"/>
+    <col min="4" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="73.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -682,7 +752,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -712,7 +782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -742,7 +812,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -772,7 +842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -799,7 +869,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -826,7 +896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -853,7 +923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -880,7 +950,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -907,12 +977,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -934,12 +1004,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -961,12 +1031,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -988,12 +1058,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1015,12 +1085,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1042,12 +1112,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1069,12 +1139,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1096,12 +1166,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1123,12 +1193,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1150,12 +1220,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1177,12 +1247,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1204,12 +1274,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C21" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1231,12 +1301,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1258,12 +1328,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C23" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1281,16 +1351,16 @@
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_022.ttl</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C24" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1308,46 +1378,108 @@
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_023.ttl</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="G24" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="6" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_024</v>
+      </c>
+      <c r="D25" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_024.vpp</v>
+      </c>
+      <c r="E25" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_024.json</v>
+      </c>
+      <c r="F25" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_024.ttl</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="6" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_025</v>
+      </c>
+      <c r="D26" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_025.vpp</v>
+      </c>
+      <c r="E26" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_025.json</v>
+      </c>
+      <c r="F26" s="6" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_025.ttl</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A24">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  <conditionalFormatting sqref="A2:A26">
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H24">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="G2:H26">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H24" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H26" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
       <formula1>"Done,TBD"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
test 029 inputs fixed
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5042CFCA-7A0C-470A-9782-9908781A04B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B1FB00-7BF7-4EF8-B60F-825DAE96A0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>#</t>
   </si>
@@ -135,22 +135,13 @@
     <t>022 + multiple different properties for attributes</t>
   </si>
   <si>
-    <t>add generalization</t>
-  </si>
-  <si>
     <t>add relation</t>
   </si>
   <si>
-    <t>add enumerations</t>
-  </si>
-  <si>
     <t>add subsets and redefines to properties</t>
   </si>
   <si>
     <t>add stereotypes for properties</t>
-  </si>
-  <si>
-    <t>add text box, notes, and comments</t>
   </si>
   <si>
     <t>023 + added attributes's stereotypes (single, valid, invalid, multiple, etc.) and meta-properties</t>
@@ -783,7 +774,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,7 +1450,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C25" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1486,7 +1477,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C26" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1513,7 +1504,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C27" s="6" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1542,7 +1533,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C28" s="6" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1571,7 +1562,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C29" s="6" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1589,7 +1580,9 @@
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_028.ttl</v>
       </c>
-      <c r="G29" s="6"/>
+      <c r="G29" t="s">
+        <v>9</v>
+      </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
     </row>
@@ -1598,7 +1591,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C30" s="6" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
@@ -1622,32 +1615,17 @@
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all tests working up to 46
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDB9E13-D8F6-4C05-9C3A-05C7BBFE516B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC7F9D7-6801-4437-954C-E6BDD4E28F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Vocabulary" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="209">
   <si>
     <t>#</t>
   </si>
@@ -639,6 +638,21 @@
   </si>
   <si>
     <t>040 + diagram inside the class from 040</t>
+  </si>
+  <si>
+    <t>017 + language tag</t>
+  </si>
+  <si>
+    <t>025 + language tag</t>
+  </si>
+  <si>
+    <t>029 + language tag</t>
+  </si>
+  <si>
+    <t>036 + language tag</t>
+  </si>
+  <si>
+    <t>041 + language tag</t>
   </si>
 </sst>
 </file>
@@ -718,7 +732,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -811,12 +825,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i/>
@@ -839,6 +847,42 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -853,26 +897,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I42" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="A1:I42" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I47" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:I47" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{B2169228-FA5D-41A3-ABA5-DC9D70D992D5}" name="Description"/>
-    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="15">
+    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="13">
       <calculatedColumnFormula>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="14">
+    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="12">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".vpp"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="13">
+    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="11">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".json"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="12">
+    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="10">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".ttl"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -883,7 +927,7 @@
   <autoFilter ref="A1:B66" xr:uid="{88DCFEC6-8E1A-4F00-80F3-4B8E00C98104}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4BBB0CEF-AE77-44B8-B4E4-835459C6A400}" name="USED"/>
-    <tableColumn id="2" xr3:uid="{605D6E5A-92F1-4F24-9A6C-40690742E0DF}" name="Used and exists" dataDxfId="8">
+    <tableColumn id="2" xr3:uid="{605D6E5A-92F1-4F24-9A6C-40690742E0DF}" name="Used and exists" dataDxfId="20">
       <calculatedColumnFormula>IF(ISERROR(VLOOKUP(Tabela1[[#This Row],[USED]],Tabela2[EXISTS],1,FALSE)),0,1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -899,7 +943,7 @@
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{33CEF012-F496-4BF4-82E7-578E21A4612F}" name="EXISTS"/>
-    <tableColumn id="2" xr3:uid="{423088D0-C022-4C9D-9FB6-40EAA00E6D27}" name="Exists and used" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{423088D0-C022-4C9D-9FB6-40EAA00E6D27}" name="Exists and used" dataDxfId="19">
       <calculatedColumnFormula>IF(ISERROR(VLOOKUP(Tabela2[[#This Row],[EXISTS]],Tabela1[[#All],[USED]],1,FALSE)),0,1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{24760A67-946D-489B-878D-8394454EE873}" name="Justified"/>
@@ -1219,10 +1263,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2359,33 +2403,179 @@
       <c r="B42" t="s">
         <v>203</v>
       </c>
-      <c r="C42" s="5" t="str">
+      <c r="C42" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_041</v>
       </c>
-      <c r="D42" s="5" t="str">
+      <c r="D42" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_041.vpp</v>
       </c>
-      <c r="E42" s="5" t="str">
+      <c r="E42" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_041.json</v>
       </c>
-      <c r="F42" s="5" t="str">
+      <c r="F42" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_041.ttl</v>
       </c>
       <c r="G42" t="s">
         <v>9</v>
       </c>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>204</v>
+      </c>
+      <c r="C43" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_042</v>
+      </c>
+      <c r="D43" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_042.vpp</v>
+      </c>
+      <c r="E43" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_042.json</v>
+      </c>
+      <c r="F43" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_042.ttl</v>
+      </c>
+      <c r="G43" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>205</v>
+      </c>
+      <c r="C44" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_043</v>
+      </c>
+      <c r="D44" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_043.vpp</v>
+      </c>
+      <c r="E44" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_043.json</v>
+      </c>
+      <c r="F44" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_043.ttl</v>
+      </c>
+      <c r="G44" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>206</v>
+      </c>
+      <c r="C45" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_044</v>
+      </c>
+      <c r="D45" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_044.vpp</v>
+      </c>
+      <c r="E45" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_044.json</v>
+      </c>
+      <c r="F45" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_044.ttl</v>
+      </c>
+      <c r="G45" t="s">
+        <v>9</v>
+      </c>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>207</v>
+      </c>
+      <c r="C46" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_045</v>
+      </c>
+      <c r="D46" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_045.vpp</v>
+      </c>
+      <c r="E46" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_045.json</v>
+      </c>
+      <c r="F46" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_045.ttl</v>
+      </c>
+      <c r="G46" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>208</v>
+      </c>
+      <c r="C47" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_046</v>
+      </c>
+      <c r="D47" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_046.vpp</v>
+      </c>
+      <c r="E47" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_046.json</v>
+      </c>
+      <c r="F47" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_046.ttl</v>
+      </c>
+      <c r="G47" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D58:D62">
+    <sortCondition ref="D58:D62"/>
+  </sortState>
+  <conditionalFormatting sqref="A2:A47">
     <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H42">
+  <conditionalFormatting sqref="G2:H47">
     <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
@@ -2394,7 +2584,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H42" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H47" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
       <formula1>"Done,TBD"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
new test added. minor improvements.
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC7F9D7-6801-4437-954C-E6BDD4E28F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8713253-DD9F-4552-9DB7-41111B332A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="210">
   <si>
     <t>#</t>
   </si>
@@ -653,6 +653,9 @@
   </si>
   <si>
     <t>041 + language tag</t>
+  </si>
+  <si>
+    <t>amaral2022ethical-requirements</t>
   </si>
 </sst>
 </file>
@@ -732,7 +735,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -825,6 +828,12 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i/>
@@ -847,42 +856,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -897,26 +870,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I47" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A1:I47" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I48" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A1:I48" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{B2169228-FA5D-41A3-ABA5-DC9D70D992D5}" name="Description"/>
-    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="13">
+    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="15">
       <calculatedColumnFormula>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="12">
+    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="14">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".vpp"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="13">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".json"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="10">
+    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="12">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".ttl"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -927,7 +900,7 @@
   <autoFilter ref="A1:B66" xr:uid="{88DCFEC6-8E1A-4F00-80F3-4B8E00C98104}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4BBB0CEF-AE77-44B8-B4E4-835459C6A400}" name="USED"/>
-    <tableColumn id="2" xr3:uid="{605D6E5A-92F1-4F24-9A6C-40690742E0DF}" name="Used and exists" dataDxfId="20">
+    <tableColumn id="2" xr3:uid="{605D6E5A-92F1-4F24-9A6C-40690742E0DF}" name="Used and exists" dataDxfId="8">
       <calculatedColumnFormula>IF(ISERROR(VLOOKUP(Tabela1[[#This Row],[USED]],Tabela2[EXISTS],1,FALSE)),0,1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -943,7 +916,7 @@
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{33CEF012-F496-4BF4-82E7-578E21A4612F}" name="EXISTS"/>
-    <tableColumn id="2" xr3:uid="{423088D0-C022-4C9D-9FB6-40EAA00E6D27}" name="Exists and used" dataDxfId="19">
+    <tableColumn id="2" xr3:uid="{423088D0-C022-4C9D-9FB6-40EAA00E6D27}" name="Exists and used" dataDxfId="7">
       <calculatedColumnFormula>IF(ISERROR(VLOOKUP(Tabela2[[#This Row],[EXISTS]],Tabela1[[#All],[USED]],1,FALSE)),0,1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{24760A67-946D-489B-878D-8394454EE873}" name="Justified"/>
@@ -1263,10 +1236,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2430,27 +2403,25 @@
       <c r="B43" t="s">
         <v>204</v>
       </c>
-      <c r="C43" s="5" t="str">
+      <c r="C43" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_042</v>
       </c>
-      <c r="D43" s="5" t="str">
+      <c r="D43" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_042.vpp</v>
       </c>
-      <c r="E43" s="5" t="str">
+      <c r="E43" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_042.json</v>
       </c>
-      <c r="F43" s="5" t="str">
+      <c r="F43" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_042.ttl</v>
       </c>
       <c r="G43" t="s">
         <v>9</v>
       </c>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
@@ -2459,27 +2430,25 @@
       <c r="B44" t="s">
         <v>205</v>
       </c>
-      <c r="C44" s="5" t="str">
+      <c r="C44" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_043</v>
       </c>
-      <c r="D44" s="5" t="str">
+      <c r="D44" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_043.vpp</v>
       </c>
-      <c r="E44" s="5" t="str">
+      <c r="E44" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_043.json</v>
       </c>
-      <c r="F44" s="5" t="str">
+      <c r="F44" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_043.ttl</v>
       </c>
       <c r="G44" t="s">
         <v>9</v>
       </c>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
@@ -2488,27 +2457,25 @@
       <c r="B45" t="s">
         <v>206</v>
       </c>
-      <c r="C45" s="5" t="str">
+      <c r="C45" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_044</v>
       </c>
-      <c r="D45" s="5" t="str">
+      <c r="D45" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_044.vpp</v>
       </c>
-      <c r="E45" s="5" t="str">
+      <c r="E45" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_044.json</v>
       </c>
-      <c r="F45" s="5" t="str">
+      <c r="F45" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_044.ttl</v>
       </c>
       <c r="G45" t="s">
         <v>9</v>
       </c>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
@@ -2517,27 +2484,25 @@
       <c r="B46" t="s">
         <v>207</v>
       </c>
-      <c r="C46" s="5" t="str">
+      <c r="C46" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_045</v>
       </c>
-      <c r="D46" s="5" t="str">
+      <c r="D46" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_045.vpp</v>
       </c>
-      <c r="E46" s="5" t="str">
+      <c r="E46" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_045.json</v>
       </c>
-      <c r="F46" s="5" t="str">
+      <c r="F46" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_045.ttl</v>
       </c>
       <c r="G46" t="s">
         <v>9</v>
       </c>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
@@ -2546,36 +2511,61 @@
       <c r="B47" t="s">
         <v>208</v>
       </c>
-      <c r="C47" s="5" t="str">
+      <c r="C47" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_046</v>
       </c>
-      <c r="D47" s="5" t="str">
+      <c r="D47" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_046.vpp</v>
       </c>
-      <c r="E47" s="5" t="str">
+      <c r="E47" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_046.json</v>
       </c>
-      <c r="F47" s="5" t="str">
+      <c r="F47" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_046.ttl</v>
       </c>
       <c r="G47" t="s">
         <v>9</v>
       </c>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>209</v>
+      </c>
+      <c r="C48" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_047</v>
+      </c>
+      <c r="D48" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_047.vpp</v>
+      </c>
+      <c r="E48" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_047.json</v>
+      </c>
+      <c r="F48" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_047.ttl</v>
+      </c>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D58:D62">
     <sortCondition ref="D58:D62"/>
   </sortState>
-  <conditionalFormatting sqref="A2:A47">
+  <conditionalFormatting sqref="A2:A48">
     <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H47">
+  <conditionalFormatting sqref="G2:H48">
     <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
@@ -2584,7 +2574,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H47" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H48" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
       <formula1>"Done,TBD"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
treating new metamodel definitions
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB59E648-902C-4F7A-A2BE-7D0C1EA94DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E30EDDE-5C2E-43C7-B7E6-4BABD21CC148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="213">
   <si>
     <t>#</t>
   </si>
@@ -659,6 +659,12 @@
   </si>
   <si>
     <t>sales2018cover</t>
+  </si>
+  <si>
+    <t>isExtensional and isPowertype possibilites</t>
+  </si>
+  <si>
+    <t>Used to test the validation function.</t>
   </si>
 </sst>
 </file>
@@ -873,8 +879,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I49" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="A1:I49" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I50" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A1:I50" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{B2169228-FA5D-41A3-ABA5-DC9D70D992D5}" name="Description"/>
@@ -1239,10 +1245,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2568,36 +2574,63 @@
       <c r="B49" t="s">
         <v>210</v>
       </c>
-      <c r="C49" s="5" t="str">
+      <c r="C49" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_048</v>
       </c>
-      <c r="D49" s="5" t="str">
+      <c r="D49" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_048.vpp</v>
       </c>
-      <c r="E49" s="5" t="str">
+      <c r="E49" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_048.json</v>
       </c>
-      <c r="F49" s="5" t="str">
+      <c r="F49" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_048.ttl</v>
       </c>
       <c r="G49" t="s">
         <v>9</v>
       </c>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>211</v>
+      </c>
+      <c r="C50" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_049</v>
+      </c>
+      <c r="D50" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_049.vpp</v>
+      </c>
+      <c r="E50" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_049.json</v>
+      </c>
+      <c r="F50" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_049.ttl</v>
+      </c>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5" t="s">
+        <v>212</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D58:D62">
     <sortCondition ref="D58:D62"/>
   </sortState>
-  <conditionalFormatting sqref="A2:A49">
+  <conditionalFormatting sqref="A2:A50">
     <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H49">
+  <conditionalFormatting sqref="G2:H50">
     <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
@@ -2606,7 +2639,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H49" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H50" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
       <formula1>"Done,TBD"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
finished set default values
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E30EDDE-5C2E-43C7-B7E6-4BABD21CC148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E4964C-EF7A-471E-98E1-267186EC022F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="218">
   <si>
     <t>#</t>
   </si>
@@ -665,6 +665,21 @@
   </si>
   <si>
     <t>Used to test the validation function.</t>
+  </si>
+  <si>
+    <t>diverse attributes with diferent settings</t>
+  </si>
+  <si>
+    <t>050 manually modified substituting attributes values from true to null</t>
+  </si>
+  <si>
+    <t>050 manually modified substituting attributes values from false to null</t>
+  </si>
+  <si>
+    <t>052 manually modified substituting attributes values from true to null</t>
+  </si>
+  <si>
+    <t>Used to test "set defaults"</t>
   </si>
 </sst>
 </file>
@@ -744,7 +759,97 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -879,26 +984,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I50" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="A1:I50" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}" name="Table1" displayName="Table1" ref="A1:I54" totalsRowShown="0" headerRowDxfId="26">
+  <autoFilter ref="A1:I54" xr:uid="{1D241AED-850D-4E6C-B2FC-D5E7EBEE2370}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{05DE13E7-73E0-4768-BF58-1CA8491F345C}" name="#" dataDxfId="25"/>
     <tableColumn id="2" xr3:uid="{B2169228-FA5D-41A3-ABA5-DC9D70D992D5}" name="Description"/>
-    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="15">
+    <tableColumn id="6" xr3:uid="{A43D3431-0F9F-4E87-A0C5-980D3042890F}" name="Base" dataDxfId="24">
       <calculatedColumnFormula>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="14">
+    <tableColumn id="7" xr3:uid="{2CD594D4-C36F-40A0-9065-78092B5D8386}" name="VPP" dataDxfId="23">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".vpp"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="13">
+    <tableColumn id="3" xr3:uid="{1E297AAE-4CDA-48FD-8E82-AF15FBA289A4}" name="JSON" dataDxfId="22">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".json"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="12">
+    <tableColumn id="4" xr3:uid="{99F5952E-22D3-4FBD-AC8B-615FD3C9784F}" name="TTL" dataDxfId="21">
       <calculatedColumnFormula>Table1[[#This Row],[Base]]&amp;".ttl"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{76CACE86-2861-4D01-8CD1-5BDB869DC29A}" name="json2graph" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{56E522DA-3787-4AA9-AB64-4A5CAB2EB622}" name="graph2json" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{32870A57-9DC3-41D9-AEE1-E457DF450E6D}" name="Comments" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -909,7 +1014,7 @@
   <autoFilter ref="A1:B66" xr:uid="{88DCFEC6-8E1A-4F00-80F3-4B8E00C98104}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4BBB0CEF-AE77-44B8-B4E4-835459C6A400}" name="USED"/>
-    <tableColumn id="2" xr3:uid="{605D6E5A-92F1-4F24-9A6C-40690742E0DF}" name="Used and exists" dataDxfId="8">
+    <tableColumn id="2" xr3:uid="{605D6E5A-92F1-4F24-9A6C-40690742E0DF}" name="Used and exists" dataDxfId="17">
       <calculatedColumnFormula>IF(ISERROR(VLOOKUP(Tabela1[[#This Row],[USED]],Tabela2[EXISTS],1,FALSE)),0,1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -925,7 +1030,7 @@
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{33CEF012-F496-4BF4-82E7-578E21A4612F}" name="EXISTS"/>
-    <tableColumn id="2" xr3:uid="{423088D0-C022-4C9D-9FB6-40EAA00E6D27}" name="Exists and used" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{423088D0-C022-4C9D-9FB6-40EAA00E6D27}" name="Exists and used" dataDxfId="16">
       <calculatedColumnFormula>IF(ISERROR(VLOOKUP(Tabela2[[#This Row],[EXISTS]],Tabela1[[#All],[USED]],1,FALSE)),0,1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{24760A67-946D-489B-878D-8394454EE873}" name="Justified"/>
@@ -1245,10 +1350,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2601,45 +2706,170 @@
       <c r="B50" t="s">
         <v>211</v>
       </c>
-      <c r="C50" s="5" t="str">
+      <c r="C50" t="str">
         <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
         <v>test_049</v>
       </c>
-      <c r="D50" s="5" t="str">
+      <c r="D50" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
         <v>test_049.vpp</v>
       </c>
-      <c r="E50" s="5" t="str">
+      <c r="E50" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".json"</f>
         <v>test_049.json</v>
       </c>
-      <c r="F50" s="5" t="str">
+      <c r="F50" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_049.ttl</v>
       </c>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5" t="s">
+      <c r="G50" t="s">
+        <v>9</v>
+      </c>
+      <c r="I50" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>213</v>
+      </c>
+      <c r="C51" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_050</v>
+      </c>
+      <c r="D51" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_050.vpp</v>
+      </c>
+      <c r="E51" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_050.json</v>
+      </c>
+      <c r="F51" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_050.ttl</v>
+      </c>
+      <c r="G51" t="s">
+        <v>9</v>
+      </c>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>214</v>
+      </c>
+      <c r="C52" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_051</v>
+      </c>
+      <c r="D52" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_051.vpp</v>
+      </c>
+      <c r="E52" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_051.json</v>
+      </c>
+      <c r="F52" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_051.ttl</v>
+      </c>
+      <c r="G52" t="s">
+        <v>9</v>
+      </c>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>215</v>
+      </c>
+      <c r="C53" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_052</v>
+      </c>
+      <c r="D53" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_052.vpp</v>
+      </c>
+      <c r="E53" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_052.json</v>
+      </c>
+      <c r="F53" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_052.ttl</v>
+      </c>
+      <c r="G53" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>216</v>
+      </c>
+      <c r="C54" s="5" t="str">
+        <f>"test_"&amp;TEXT(Table1[[#This Row],['#]],"000")</f>
+        <v>test_053</v>
+      </c>
+      <c r="D54" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".vpp"</f>
+        <v>test_053.vpp</v>
+      </c>
+      <c r="E54" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".json"</f>
+        <v>test_053.json</v>
+      </c>
+      <c r="F54" s="5" t="str">
+        <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
+        <v>test_053.ttl</v>
+      </c>
+      <c r="G54" t="s">
+        <v>9</v>
+      </c>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D58:D62">
     <sortCondition ref="D58:D62"/>
   </sortState>
-  <conditionalFormatting sqref="A2:A50">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+  <conditionalFormatting sqref="A2:A54">
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H50">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+  <conditionalFormatting sqref="G2:H54">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H50" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H54" xr:uid="{730C37A3-AAC7-4218-8A22-535273AF5656}">
       <formula1>"Done,TBD"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4346,7 +4576,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F86">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
included tests 50 to 53 (not validated yet)
</commit_message>
<xml_diff>
--- a/tests/test_files/List of Tests.xlsx
+++ b/tests/test_files/List of Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Dev\Work\ontouml-json2graph\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E4964C-EF7A-471E-98E1-267186EC022F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FB4309-A98E-4768-8E36-5FF57D92A80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{337D8CB5-42E6-48D8-9B41-5D7BCCB0FAFA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="218">
   <si>
     <t>#</t>
   </si>
@@ -1353,7 +1353,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2783,9 +2783,6 @@
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_051.ttl</v>
       </c>
-      <c r="G52" t="s">
-        <v>9</v>
-      </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5" t="s">
         <v>217</v>
@@ -2814,9 +2811,6 @@
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_052.ttl</v>
       </c>
-      <c r="G53" t="s">
-        <v>9</v>
-      </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5" t="s">
         <v>217</v>
@@ -2844,9 +2838,6 @@
       <c r="F54" s="5" t="str">
         <f>Table1[[#This Row],[Base]]&amp;".ttl"</f>
         <v>test_053.ttl</v>
-      </c>
-      <c r="G54" t="s">
-        <v>9</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="5" t="s">

</xml_diff>